<commit_message>
fixes small errors and validates xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/catch_metadata.xlsx
+++ b/data-raw/metadata/catch_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-knights-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E0E5E1-BAA8-5D4B-9006-2AA2C8A53B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67AE1C4F-7885-4843-9017-7020F7C3DD98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t>maximum</t>
-  </si>
-  <si>
-    <t>projectDescriptionID</t>
   </si>
   <si>
     <t>nominal</t>
@@ -219,6 +216,9 @@
   </si>
   <si>
     <t>2022-10-22 14:30:52</t>
+  </si>
+  <si>
+    <t>ProjectDescriptionID</t>
   </si>
 </sst>
 </file>
@@ -535,7 +535,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -612,19 +612,19 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -650,19 +650,19 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -688,33 +688,33 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="6"/>
       <c r="J4" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K4" s="6"/>
       <c r="L4" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
@@ -732,19 +732,19 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>54</v>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
@@ -770,19 +770,19 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
@@ -808,19 +808,19 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
@@ -846,19 +846,19 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -884,19 +884,19 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>47</v>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -922,19 +922,19 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="C10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -960,19 +960,19 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>59</v>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -998,19 +998,19 @@
     </row>
     <row r="12" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="E12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -1036,19 +1036,19 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="E13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -1074,28 +1074,28 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="F14" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="3"/>
@@ -1122,28 +1122,28 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>30</v>
+      <c r="C15" s="1" t="s">
+        <v>25</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="F15" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="3"/>
@@ -1170,28 +1170,28 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>32</v>
+      <c r="C16" s="1" t="s">
+        <v>25</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="F16" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="3"/>
@@ -1218,28 +1218,28 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>34</v>
+      <c r="C17" s="1" t="s">
+        <v>25</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="F17" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="3"/>
@@ -28126,13 +28126,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>

</xml_diff>

<commit_message>
updates metadata to be standard across CDFW packages
</commit_message>
<xml_diff>
--- a/data-raw/metadata/catch_metadata.xlsx
+++ b/data-raw/metadata/catch_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-knights-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67AE1C4F-7885-4843-9017-7020F7C3DD98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB76BD98-8BFA-434A-92F9-18BE61223D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -166,9 +166,6 @@
     <t>commonName</t>
   </si>
   <si>
-    <t>Common name of marked species.</t>
-  </si>
-  <si>
     <t>fishOrigin</t>
   </si>
   <si>
@@ -176,9 +173,6 @@
   </si>
   <si>
     <t>visitType</t>
-  </si>
-  <si>
-    <t>Foreign key to the CAMP ProjectDescription table. For Knight's Landing RST, projectDescriptionID = 9.</t>
   </si>
   <si>
     <t xml:space="preserve">Date and time of day associated with the trap visit. Definition varies based on visitType. </t>
@@ -203,10 +197,6 @@
     <t>run</t>
   </si>
   <si>
-    <t>Run designation assigned at a later date.  Levels = c(NA, "Winter", "Late fall", "Spring", "Fall", "Not recorded", 
-"Not applicable (n/a)")</t>
-  </si>
-  <si>
     <t>Origin/production type of the fish. Levels = c("Natural", "Hatchery", "Not recorded", "Unknown")</t>
   </si>
   <si>
@@ -219,6 +209,28 @@
   </si>
   <si>
     <t>ProjectDescriptionID</t>
+  </si>
+  <si>
+    <t>Foreign key to the CAMP ProjectDescription table. All data associated with this package will have a ProjectDescriptionID = 9.</t>
+  </si>
+  <si>
+    <t>Common name of marked species. Levels = c("Chinook salmon", "Steelhead / rainbow trout", "Unknown lamprey", 
+"River lamprey", "Pacific lamprey", "Black bullhead", "Bluegill", 
+"Threadfin shad", "Spotted bass", "Prickly sculpin", "Golden shiner", 
+"Sacramento sucker", "Inland silverside", "Mosquitofish", "Fathead minnow", 
+"Brown bullhead", "Threespine stickleback", "Unknown sunfish (Lepomis)", 
+"Largemouth bass", "Common carp", "Channel catfish", "Wakasagi / Japanese smelt", 
+"Goldfish", "Black crappie", "White crappie", "Tule perch", "Hardhead", 
+"Hitch", "Splittail", "Warmouth", "Sacramento pikeminnow", "White catfish", 
+"Striped bass", "Green sunfish", "Red shiner", "Redear sunfish", 
+"Unknown minnow", "Riffle sculpin", "Smallmouth bass", "Unknown", 
+"Yellowfin goby", "American shad", "Unknown Centrarchid", "Unknown catfish/bullhead", 
+"Unknown bass (Micropterus)", "California roach", "Sacramento perch", 
+"Unknown sculpin (Cottus)", "Other", "Unknown crappie (Pomoxis)", 
+"Speckled dace", "Logperch", "Sacramento blackfish")</t>
+  </si>
+  <si>
+    <t>Run designation assigned at a later date.  Levels = c(NA, "Winter", "Late fall", "Spring", "Fall")</t>
   </si>
 </sst>
 </file>
@@ -535,7 +547,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -612,10 +624,10 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
@@ -691,7 +703,7 @@
         <v>35</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>36</v>
@@ -714,7 +726,7 @@
         <v>44</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
@@ -732,10 +744,10 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -770,10 +782,10 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -808,10 +820,10 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
@@ -887,7 +899,7 @@
         <v>45</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
@@ -960,10 +972,10 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
@@ -998,10 +1010,10 @@
     </row>
     <row r="12" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
@@ -1036,10 +1048,10 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
adds trap_start_date, and trap_end_date metadata, adds code to check na values
</commit_message>
<xml_diff>
--- a/data-raw/metadata/catch_metadata.xlsx
+++ b/data-raw/metadata/catch_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-knights-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0352F5-19CF-4099-9BDC-8076416A5296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05F0CB9-E7A0-459A-B9E6-AA40B50764BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5540" yWindow="1290" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20520" yWindow="990" windowWidth="15765" windowHeight="14295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="71">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -241,6 +241,21 @@
   <si>
     <t>2023-12-25 10:30:12</t>
   </si>
+  <si>
+    <t>trap_start_date</t>
+  </si>
+  <si>
+    <t>Start date and time of a trapping period. Derived from visitTime and visitTime2 fields, adjusted based on the visitType field</t>
+  </si>
+  <si>
+    <t>trap</t>
+  </si>
+  <si>
+    <t>trap_end_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> End date and time of a trapping period. Derived from visitTime and visitTime2 fields, adjusted based on the visitType field</t>
+  </si>
 </sst>
 </file>
 
@@ -313,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -337,6 +352,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,8 +579,8 @@
   <dimension ref="A1:Z976"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1330,19 +1354,35 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="4"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
+      <c r="A19" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K19" s="12"/>
+      <c r="L19" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="M19" s="13" t="s">
+        <v>65</v>
+      </c>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
@@ -1358,19 +1398,35 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="4"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
+      <c r="A20" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K20" s="12"/>
+      <c r="L20" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="M20" s="13" t="s">
+        <v>65</v>
+      </c>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>

</xml_diff>

<commit_message>
updates fields domain in metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/catch_metadata.xlsx
+++ b/data-raw/metadata/catch_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-knights-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F06F6C0-F8EA-44B3-B887-07A06760B0EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E79300-7909-4473-8959-3DD4B317F999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="2050" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -581,9 +581,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z976"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -666,7 +666,7 @@
         <v>60</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
updates min/max values on metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/catch_metadata.xlsx
+++ b/data-raw/metadata/catch_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-knights-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E79300-7909-4473-8959-3DD4B317F999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F82557E-8FEC-4CD8-99AD-B41D9049CB50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="2050" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21405" yWindow="1470" windowWidth="18600" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="70">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -205,9 +205,6 @@
 "Adult", "YOY (young of the year)")</t>
   </si>
   <si>
-    <t>2022-10-22 14:30:52</t>
-  </si>
-  <si>
     <t>ProjectDescriptionID</t>
   </si>
   <si>
@@ -237,9 +234,6 @@
   </si>
   <si>
     <t xml:space="preserve">Date and time of day associated with the end of trap visit. Definition varies based on visitType. </t>
-  </si>
-  <si>
-    <t>2023-12-25 10:30:12</t>
   </si>
   <si>
     <t>trap_start_date</t>
@@ -581,9 +575,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z976"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -660,10 +654,10 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>17</v>
@@ -672,7 +666,7 @@
         <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -762,7 +756,7 @@
         <v>44</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
@@ -780,10 +774,10 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>36</v>
@@ -806,7 +800,7 @@
         <v>44</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -979,7 +973,7 @@
         <v>45</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>
@@ -1055,7 +1049,7 @@
         <v>55</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
@@ -1358,10 +1352,10 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>36</v>
@@ -1384,7 +1378,7 @@
         <v>44</v>
       </c>
       <c r="M19" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
@@ -1402,10 +1396,10 @@
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>36</v>
@@ -1428,7 +1422,7 @@
         <v>44</v>
       </c>
       <c r="M20" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
@@ -28287,10 +28281,10 @@
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>

</xml_diff>